<commit_message>
Modificando a lista de parâmetros e a base de dados
</commit_message>
<xml_diff>
--- a/Base de dados inicial.xlsx
+++ b/Base de dados inicial.xlsx
@@ -5,36 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbdfa6a349ea30/ENG_Q/PIBITI/Otimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aline\Documents\Graduação\PIBITI\PIBITI-Compartilhado\PIBITI-Otimizacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{DBB55728-F720-49C6-AB1C-AF102F5CFD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0715C13F-E4C0-4B39-9733-987DED6761EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1367F85-CAB9-42DD-94BB-82543D44C9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CA415204-792B-4894-BF4B-2B5BE2F0893D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{CA415204-792B-4894-BF4B-2B5BE2F0893D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Variedades</t>
   </si>
@@ -42,9 +33,6 @@
     <t>Pol</t>
   </si>
   <si>
-    <t>Cor</t>
-  </si>
-  <si>
     <t>Var1</t>
   </si>
   <si>
@@ -69,26 +57,33 @@
     <t>pH (adimensional)</t>
   </si>
   <si>
-    <t>Ponto de Fusão (ºC)</t>
-  </si>
-  <si>
-    <t>Ponto de ebulição (ºC)</t>
-  </si>
-  <si>
-    <t>Brix (ºBx)</t>
-  </si>
-  <si>
-    <t>Viscosidade (10^6Pa.s)</t>
-  </si>
-  <si>
-    <t>variedade(nome,custo,pH,pf,pe,brix,pol,visc,cor)</t>
+    <t>Pureza (%)</t>
+  </si>
+  <si>
+    <t>ATR (%)</t>
+  </si>
+  <si>
+    <t>AR (%)</t>
+  </si>
+  <si>
+    <t>Fibra (%)</t>
+  </si>
+  <si>
+    <t>variedade(nome,custo,pH,pol,pureza, atr, ar, fibra)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,22 +130,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182373A1-0484-4FE9-836E-45CE3B1D29BF}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -478,217 +485,202 @@
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G2" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="G4" s="5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.11459999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="5">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.12889999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.1201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="G7" s="5">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.1178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-114.1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>78.400000000000006</v>
-      </c>
-      <c r="F2" s="1">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1194</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5.4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-110</v>
-      </c>
-      <c r="E3" s="1">
-        <v>81</v>
-      </c>
-      <c r="F3" s="1">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5.8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>-112</v>
-      </c>
-      <c r="E4" s="1">
-        <v>80</v>
-      </c>
-      <c r="F4" s="1">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1">
-        <v>21</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1860</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-109</v>
-      </c>
-      <c r="E5" s="1">
-        <v>79</v>
-      </c>
-      <c r="F5" s="1">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1150</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-108</v>
-      </c>
-      <c r="E6" s="1">
-        <v>85</v>
-      </c>
-      <c r="F6" s="1">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1220</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="C7" s="1">
-        <v>7.2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-106</v>
-      </c>
-      <c r="E7" s="1">
-        <v>86</v>
-      </c>
-      <c r="F7" s="1">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1">
-        <v>15</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1920</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D10:F10"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>